<commit_message>
DatabaseExport.sql dump with data without absences.
</commit_message>
<xml_diff>
--- a/TeamWork.xlsx
+++ b/TeamWork.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_NBU\III_KURS\6BD\my-school\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C2C1EFD-524E-4288-A99A-1FA45926219C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDCF062-1AED-4964-A8BA-60433DAD32EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{41B0A16E-193E-4D5D-9742-942A5EE57AB4}"/>
+    <workbookView xWindow="6048" yWindow="612" windowWidth="16956" windowHeight="11628" xr2:uid="{41B0A16E-193E-4D5D-9742-942A5EE57AB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
   <si>
     <t>Лъчо</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Users&amp;Role</t>
+  </si>
+  <si>
+    <t>Подготовка на БД</t>
   </si>
 </sst>
 </file>
@@ -530,7 +533,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -752,10 +755,14 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+      <c r="D20" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21"/>

</xml_diff>